<commit_message>
Added code for reading the dataset
</commit_message>
<xml_diff>
--- a/EBayMobileAutomationFramework/src/test/resources/TestData.xlsx
+++ b/EBayMobileAutomationFramework/src/test/resources/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBED861-9C69-4CD8-AC1B-C5AE9176A481}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E754779-ECAA-41C1-AA9B-7A1E2BE297F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Item</t>
-  </si>
-  <si>
     <t>64 inch TV</t>
   </si>
   <si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>Queen Bed</t>
+  </si>
+  <si>
+    <t>Item To Search</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,27 +380,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>